<commit_message>
Fill all report-checklist fields
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/MEDICAL_80/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/MEDICAL_80/1.0/report-checklist.xlsx
@@ -21,11 +21,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$383</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="oXWj5iU3LtnvLpdhFqszSz/X91q3fG5U5zC5TJKtiGw="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -61,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="893">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4685,6 +4680,24 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.985ca4b25548f895283e6dcc2edc30398af0a82157187c67bfe4ea758586423a.5cc73a2b83^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: Campo token JWT non valido.</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: il servizio ha impiegato troppo tempo a rispondere.</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: Errore semantico.</t>
+  </si>
+  <si>
+    <t>Errore validazione CDA: Errore vocabolario.</t>
+  </si>
+  <si>
+    <t>In questo caso il documento viene comunque fatto firmare e pubblicato. Si potrà decidere con il cliente se impostare re-invii automatici o manuali.</t>
+  </si>
+  <si>
+    <t>Si potrà decidere con il cliente se rendere l'errore bloccante, e quindi chiedere di correggere il dato all'operatore di back-office prima di procedere con la firma e con la pubblicazione, oppure proseguire comunque con la firma e pubblicazione del documento ed eventualmente correggere successivamente il problema con un referto sostitutivo.</t>
   </si>
 </sst>
 </file>
@@ -5007,7 +5020,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5119,6 +5132,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7605,7 +7630,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J362" sqref="J362"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -7794,7 +7819,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="37.5">
+    <row r="9" spans="1:20" ht="38.25" thickBot="1">
       <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
@@ -8026,7 +8051,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="150">
+    <row r="15" spans="1:20" ht="150.75" thickBot="1">
       <c r="A15" s="20">
         <v>6</v>
       </c>
@@ -8063,14 +8088,16 @@
       <c r="N15" s="25"/>
       <c r="O15" s="25"/>
       <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
+      <c r="Q15" s="46" t="s">
+        <v>846</v>
+      </c>
       <c r="R15" s="26"/>
       <c r="S15" s="27"/>
       <c r="T15" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="150">
+    <row r="16" spans="1:20" ht="150.75" thickBot="1">
       <c r="A16" s="20">
         <v>7</v>
       </c>
@@ -8108,7 +8135,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="150">
+    <row r="17" spans="1:20" ht="150.75" thickBot="1">
       <c r="A17" s="20">
         <v>8</v>
       </c>
@@ -8146,7 +8173,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="150">
+    <row r="18" spans="1:20" ht="150.75" thickBot="1">
       <c r="A18" s="20">
         <v>9</v>
       </c>
@@ -8762,7 +8789,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="150">
+    <row r="36" spans="1:20" ht="210.75" thickBot="1">
       <c r="A36" s="20">
         <v>29</v>
       </c>
@@ -8794,19 +8821,31 @@
         <v>139</v>
       </c>
       <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="25"/>
+      <c r="L36" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="M36" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="N36" s="48" t="s">
+        <v>887</v>
+      </c>
+      <c r="O36" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="P36" s="49" t="s">
+        <v>892</v>
+      </c>
+      <c r="Q36" s="47" t="s">
+        <v>846</v>
+      </c>
       <c r="R36" s="26"/>
       <c r="S36" s="27"/>
       <c r="T36" s="28" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="150" hidden="1">
+    <row r="37" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A37" s="20">
         <v>30</v>
       </c>
@@ -9044,7 +9083,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="165">
+    <row r="44" spans="1:20" ht="210.75" thickBot="1">
       <c r="A44" s="20">
         <v>37</v>
       </c>
@@ -9076,19 +9115,31 @@
         <v>139</v>
       </c>
       <c r="K44" s="25"/>
-      <c r="L44" s="25"/>
-      <c r="M44" s="25"/>
-      <c r="N44" s="25"/>
-      <c r="O44" s="25"/>
-      <c r="P44" s="25"/>
-      <c r="Q44" s="25"/>
+      <c r="L44" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="M44" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="N44" s="48" t="s">
+        <v>887</v>
+      </c>
+      <c r="O44" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="P44" s="49" t="s">
+        <v>892</v>
+      </c>
+      <c r="Q44" s="48" t="s">
+        <v>846</v>
+      </c>
       <c r="R44" s="26"/>
       <c r="S44" s="27"/>
       <c r="T44" s="28" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="165" hidden="1">
+    <row r="45" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A45" s="20">
         <v>38</v>
       </c>
@@ -9328,7 +9379,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="60">
+    <row r="52" spans="1:20" ht="60.75" thickBot="1">
       <c r="A52" s="20">
         <v>45</v>
       </c>
@@ -9356,12 +9407,24 @@
         <v>139</v>
       </c>
       <c r="K52" s="25"/>
-      <c r="L52" s="25"/>
-      <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="25"/>
-      <c r="P52" s="25"/>
-      <c r="Q52" s="25"/>
+      <c r="L52" s="48" t="s">
+        <v>848</v>
+      </c>
+      <c r="M52" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="N52" s="48" t="s">
+        <v>888</v>
+      </c>
+      <c r="O52" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="P52" s="49" t="s">
+        <v>891</v>
+      </c>
+      <c r="Q52" s="48" t="s">
+        <v>846</v>
+      </c>
       <c r="R52" s="26" t="s">
         <v>139</v>
       </c>
@@ -9960,7 +10023,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="120">
+    <row r="70" spans="1:20" ht="120.75" thickBot="1">
       <c r="A70" s="20">
         <v>63</v>
       </c>
@@ -9986,7 +10049,7 @@
       <c r="K70" s="25" t="s">
         <v>865</v>
       </c>
-      <c r="L70" s="25"/>
+      <c r="L70" s="48"/>
       <c r="M70" s="25"/>
       <c r="N70" s="25"/>
       <c r="O70" s="25"/>
@@ -9998,7 +10061,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="120">
+    <row r="71" spans="1:20" ht="120.75" thickBot="1">
       <c r="A71" s="20">
         <v>64</v>
       </c>
@@ -10024,7 +10087,7 @@
       <c r="K71" s="25" t="s">
         <v>866</v>
       </c>
-      <c r="L71" s="25"/>
+      <c r="L71" s="48"/>
       <c r="M71" s="25"/>
       <c r="N71" s="25"/>
       <c r="O71" s="25"/>
@@ -10036,7 +10099,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="120.75" thickBot="1">
+    <row r="72" spans="1:20" ht="210.75" thickBot="1">
       <c r="A72" s="20">
         <v>65</v>
       </c>
@@ -10068,12 +10131,24 @@
         <v>139</v>
       </c>
       <c r="K72" s="25"/>
-      <c r="L72" s="25"/>
-      <c r="M72" s="25"/>
-      <c r="N72" s="25"/>
-      <c r="O72" s="25"/>
-      <c r="P72" s="25"/>
-      <c r="Q72" s="25"/>
+      <c r="L72" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="M72" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="N72" s="48" t="s">
+        <v>889</v>
+      </c>
+      <c r="O72" s="48" t="s">
+        <v>848</v>
+      </c>
+      <c r="P72" s="49" t="s">
+        <v>892</v>
+      </c>
+      <c r="Q72" s="48" t="s">
+        <v>846</v>
+      </c>
       <c r="R72" s="26"/>
       <c r="S72" s="27"/>
       <c r="T72" s="28" t="s">
@@ -10106,7 +10181,7 @@
       <c r="K73" s="25" t="s">
         <v>870</v>
       </c>
-      <c r="L73" s="25"/>
+      <c r="L73" s="48"/>
       <c r="M73" s="25"/>
       <c r="N73" s="25"/>
       <c r="O73" s="25"/>
@@ -10118,7 +10193,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="120.75" thickBot="1">
+    <row r="74" spans="1:20" ht="210.75" thickBot="1">
       <c r="A74" s="20">
         <v>67</v>
       </c>
@@ -10150,19 +10225,31 @@
         <v>139</v>
       </c>
       <c r="K74" s="25"/>
-      <c r="L74" s="25"/>
-      <c r="M74" s="25"/>
-      <c r="N74" s="25"/>
-      <c r="O74" s="25"/>
-      <c r="P74" s="25"/>
-      <c r="Q74" s="25"/>
+      <c r="L74" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="M74" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="N74" s="48" t="s">
+        <v>889</v>
+      </c>
+      <c r="O74" s="48" t="s">
+        <v>848</v>
+      </c>
+      <c r="P74" s="49" t="s">
+        <v>892</v>
+      </c>
+      <c r="Q74" s="48" t="s">
+        <v>846</v>
+      </c>
       <c r="R74" s="26"/>
       <c r="S74" s="27"/>
       <c r="T74" s="28" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="120.75" thickBot="1">
+    <row r="75" spans="1:20" ht="210.75" thickBot="1">
       <c r="A75" s="20">
         <v>68</v>
       </c>
@@ -10194,19 +10281,31 @@
         <v>139</v>
       </c>
       <c r="K75" s="25"/>
-      <c r="L75" s="25"/>
-      <c r="M75" s="25"/>
-      <c r="N75" s="25"/>
-      <c r="O75" s="25"/>
-      <c r="P75" s="25"/>
-      <c r="Q75" s="25"/>
+      <c r="L75" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="M75" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="N75" s="48" t="s">
+        <v>889</v>
+      </c>
+      <c r="O75" s="48" t="s">
+        <v>848</v>
+      </c>
+      <c r="P75" s="49" t="s">
+        <v>892</v>
+      </c>
+      <c r="Q75" s="48" t="s">
+        <v>846</v>
+      </c>
       <c r="R75" s="26"/>
       <c r="S75" s="27"/>
       <c r="T75" s="28" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="120.75" thickBot="1">
+    <row r="76" spans="1:20" ht="210.75" thickBot="1">
       <c r="A76" s="20">
         <v>69</v>
       </c>
@@ -10238,19 +10337,31 @@
         <v>139</v>
       </c>
       <c r="K76" s="25"/>
-      <c r="L76" s="25"/>
-      <c r="M76" s="25"/>
-      <c r="N76" s="25"/>
-      <c r="O76" s="25"/>
-      <c r="P76" s="25"/>
-      <c r="Q76" s="25"/>
+      <c r="L76" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="M76" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="N76" s="48" t="s">
+        <v>889</v>
+      </c>
+      <c r="O76" s="48" t="s">
+        <v>848</v>
+      </c>
+      <c r="P76" s="49" t="s">
+        <v>892</v>
+      </c>
+      <c r="Q76" s="48" t="s">
+        <v>846</v>
+      </c>
       <c r="R76" s="26"/>
       <c r="S76" s="27"/>
       <c r="T76" s="28" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="120.75" thickBot="1">
+    <row r="77" spans="1:20" ht="210.75" thickBot="1">
       <c r="A77" s="20">
         <v>70</v>
       </c>
@@ -10282,12 +10393,24 @@
         <v>139</v>
       </c>
       <c r="K77" s="25"/>
-      <c r="L77" s="25"/>
-      <c r="M77" s="25"/>
-      <c r="N77" s="25"/>
-      <c r="O77" s="25"/>
-      <c r="P77" s="25"/>
-      <c r="Q77" s="25"/>
+      <c r="L77" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="M77" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="N77" s="48" t="s">
+        <v>889</v>
+      </c>
+      <c r="O77" s="48" t="s">
+        <v>848</v>
+      </c>
+      <c r="P77" s="49" t="s">
+        <v>892</v>
+      </c>
+      <c r="Q77" s="48" t="s">
+        <v>846</v>
+      </c>
       <c r="R77" s="26"/>
       <c r="S77" s="27"/>
       <c r="T77" s="28" t="s">
@@ -10320,7 +10443,7 @@
       <c r="K78" s="25" t="s">
         <v>877</v>
       </c>
-      <c r="L78" s="25"/>
+      <c r="L78" s="48"/>
       <c r="M78" s="25"/>
       <c r="N78" s="25"/>
       <c r="O78" s="25"/>
@@ -10358,7 +10481,7 @@
       <c r="K79" s="25" t="s">
         <v>877</v>
       </c>
-      <c r="L79" s="25"/>
+      <c r="L79" s="48"/>
       <c r="M79" s="25"/>
       <c r="N79" s="25"/>
       <c r="O79" s="25"/>
@@ -10370,7 +10493,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="120.75" thickBot="1">
+    <row r="80" spans="1:20" ht="210.75" thickBot="1">
       <c r="A80" s="20">
         <v>73</v>
       </c>
@@ -10402,12 +10525,24 @@
         <v>139</v>
       </c>
       <c r="K80" s="25"/>
-      <c r="L80" s="25"/>
-      <c r="M80" s="25"/>
-      <c r="N80" s="25"/>
-      <c r="O80" s="25"/>
-      <c r="P80" s="25"/>
-      <c r="Q80" s="25"/>
+      <c r="L80" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="M80" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="N80" s="48" t="s">
+        <v>890</v>
+      </c>
+      <c r="O80" s="48" t="s">
+        <v>848</v>
+      </c>
+      <c r="P80" s="49" t="s">
+        <v>892</v>
+      </c>
+      <c r="Q80" s="48" t="s">
+        <v>846</v>
+      </c>
       <c r="R80" s="26"/>
       <c r="S80" s="27"/>
       <c r="T80" s="28" t="s">
@@ -10440,7 +10575,7 @@
       <c r="K81" s="25" t="s">
         <v>877</v>
       </c>
-      <c r="L81" s="25"/>
+      <c r="L81" s="48"/>
       <c r="M81" s="25"/>
       <c r="N81" s="25"/>
       <c r="O81" s="25"/>
@@ -14974,7 +15109,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="210">
+    <row r="215" spans="1:20" ht="210.75" thickBot="1">
       <c r="A215" s="20">
         <v>208</v>
       </c>
@@ -15008,7 +15143,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="255">
+    <row r="216" spans="1:20" ht="255.75" thickBot="1">
       <c r="A216" s="20">
         <v>209</v>
       </c>
@@ -15484,7 +15619,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="240">
+    <row r="230" spans="1:20" ht="240.75" thickBot="1">
       <c r="A230" s="20">
         <v>223</v>
       </c>
@@ -18918,7 +19053,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="331" spans="1:20" ht="285">
+    <row r="331" spans="1:20" ht="285.75" thickBot="1">
       <c r="A331" s="20">
         <v>324</v>
       </c>
@@ -18952,7 +19087,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="332" spans="1:20" ht="240">
+    <row r="332" spans="1:20" ht="240.75" thickBot="1">
       <c r="A332" s="20">
         <v>325</v>
       </c>
@@ -19020,7 +19155,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="270">
+    <row r="334" spans="1:20" ht="270.75" thickBot="1">
       <c r="A334" s="20">
         <v>327</v>
       </c>
@@ -19938,7 +20073,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="361" spans="1:20" ht="255">
+    <row r="361" spans="1:20" ht="255.75" thickBot="1">
       <c r="A361" s="20">
         <v>354</v>
       </c>
@@ -19972,7 +20107,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="362" spans="1:20" ht="225">
+    <row r="362" spans="1:20" ht="225.75" thickBot="1">
       <c r="A362" s="20">
         <v>355</v>
       </c>
@@ -20485,7 +20620,9 @@
       <c r="N376" s="25"/>
       <c r="O376" s="25"/>
       <c r="P376" s="25"/>
-      <c r="Q376" s="25"/>
+      <c r="Q376" s="48" t="s">
+        <v>846</v>
+      </c>
       <c r="R376" s="26"/>
       <c r="S376" s="27"/>
       <c r="T376" s="28" t="s">
@@ -25398,11 +25535,11 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O375:O383 L10:M36 O10:O36 J38 L38:M38 O38 J19:J35 L40:M44 O40:O44 J46 L46:M46 O46 J40:J43 L48:M52 O48:O52 J10:J14 L54:M198 O54:O198 J375:J383 L375:M383 J48:J51 J54:J71 J82:J198 J73:J77 J80">
+  <dataValidations disablePrompts="1" count="4">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O375:O383 O54:O198 O10:O36 J38 L38:M38 O38 J19:J35 L10:M36 O40:O44 J46 L46:M46 O46 J40:J43 J80 O48:O52 J10:J14 L48:M52 L54:M198 J375:J383 L375:M383 J48:J51 J54:J71 J82:J198 J73:J77 L40:M44">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q10:Q36 Q38 Q40:Q44 Q46 Q48:Q52 Q54:Q198 Q375:Q383">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q10:Q36 Q38 Q40:Q44 Q46 Q54:Q198 Q48:Q52 Q375:Q383">
       <formula1>Sheet1!$A$2:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J15:J18 J36 J44 J52 J72">

</xml_diff>

<commit_message>
Ricarica test per bug workflow id non presente nei log
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/MEDICAL_80/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111LOGO80X00000/Log80_s.r.l/MEDICAL_80/1.0/report-checklist.xlsx
@@ -4577,12 +4577,6 @@
     <t>subject_application_version: 1.0</t>
   </si>
   <si>
-    <t>9c25a39758ff8419</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.d432d578260b3769f32d852d1f1fe3f24f26f5cfbe1cc19af51f5f998e152bfe.741ce9882a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>49becb6aa64f2957</t>
   </si>
   <si>
@@ -4592,9 +4586,6 @@
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>2023-09-25T12:33:25Z</t>
-  </si>
-  <si>
     <t>2023-09-25T14:37:36Z</t>
   </si>
   <si>
@@ -4604,15 +4595,6 @@
     <t>2023-09-25T14:42:45Z</t>
   </si>
   <si>
-    <t>2023-09-25T14:27:08Z</t>
-  </si>
-  <si>
-    <t>473fdcdb207f5e45</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.619c880fe6cddac388d815bfbfee642b18ed2cf033d59a177384219fcfb04aa2.c0ddb6e6a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Non sono gestiti alcuni campi opzionali nel dettaglio richiesto</t>
   </si>
   <si>
@@ -4698,6 +4680,24 @@
   </si>
   <si>
     <t>Si potrà decidere con il cliente se rendere l'errore bloccante, e quindi chiedere di correggere il dato all'operatore di back-office prima di procedere con la firma e con la pubblicazione, oppure proseguire comunque con la firma e pubblicazione del documento ed eventualmente correggere successivamente il problema con un referto sostitutivo.</t>
+  </si>
+  <si>
+    <t>2023-10-09T10:05:08Z</t>
+  </si>
+  <si>
+    <t>0391e0ba997b0a73</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.d432d578260b3769f32d852d1f1fe3f24f26f5cfbe1cc19af51f5f998e152bfe.d18dc5b57a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-09T10:15:38Z</t>
+  </si>
+  <si>
+    <t>e620b1d30a640c3f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.619c880fe6cddac388d815bfbfee642b18ed2cf033d59a177384219fcfb04aa2.bd08c78a46^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -5111,6 +5111,18 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5132,18 +5144,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7627,10 +7627,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="N362" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="P376" sqref="P376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -7668,12 +7668,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="18.75">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="37"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="41"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -7691,14 +7691,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="15.75">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="49" t="s">
         <v>849</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="41"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -7716,12 +7716,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="15.75">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="49" t="s">
         <v>850</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -7740,12 +7740,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="15.75">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49" t="s">
         <v>851</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="41"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -7763,8 +7763,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -8068,16 +8068,16 @@
         <v>59</v>
       </c>
       <c r="F15" s="23">
-        <v>45194</v>
+        <v>45208</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>857</v>
+        <v>887</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>852</v>
+        <v>888</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>853</v>
+        <v>889</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>139</v>
@@ -8088,7 +8088,7 @@
       <c r="N15" s="25"/>
       <c r="O15" s="25"/>
       <c r="P15" s="25"/>
-      <c r="Q15" s="46" t="s">
+      <c r="Q15" s="34" t="s">
         <v>846</v>
       </c>
       <c r="R15" s="26"/>
@@ -8121,7 +8121,7 @@
         <v>848</v>
       </c>
       <c r="K16" s="25" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
@@ -8159,7 +8159,7 @@
         <v>848</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
@@ -8197,7 +8197,7 @@
         <v>848</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
@@ -8809,34 +8809,34 @@
         <v>45194</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="H36" s="24" t="s">
+        <v>852</v>
+      </c>
+      <c r="I36" s="24" t="s">
         <v>854</v>
-      </c>
-      <c r="I36" s="24" t="s">
-        <v>856</v>
       </c>
       <c r="J36" s="25" t="s">
         <v>139</v>
       </c>
       <c r="K36" s="25"/>
-      <c r="L36" s="48" t="s">
+      <c r="L36" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="M36" s="48" t="s">
+      <c r="M36" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="N36" s="48" t="s">
-        <v>887</v>
-      </c>
-      <c r="O36" s="48" t="s">
+      <c r="N36" s="36" t="s">
+        <v>881</v>
+      </c>
+      <c r="O36" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="P36" s="49" t="s">
-        <v>892</v>
-      </c>
-      <c r="Q36" s="47" t="s">
+      <c r="P36" s="37" t="s">
+        <v>886</v>
+      </c>
+      <c r="Q36" s="35" t="s">
         <v>846</v>
       </c>
       <c r="R36" s="26"/>
@@ -9103,34 +9103,34 @@
         <v>45194</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="I44" s="24" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="J44" s="25" t="s">
         <v>139</v>
       </c>
       <c r="K44" s="25"/>
-      <c r="L44" s="48" t="s">
+      <c r="L44" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="M44" s="48" t="s">
+      <c r="M44" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="N44" s="48" t="s">
-        <v>887</v>
-      </c>
-      <c r="O44" s="48" t="s">
+      <c r="N44" s="36" t="s">
+        <v>881</v>
+      </c>
+      <c r="O44" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="P44" s="49" t="s">
-        <v>892</v>
-      </c>
-      <c r="Q44" s="48" t="s">
+      <c r="P44" s="37" t="s">
+        <v>886</v>
+      </c>
+      <c r="Q44" s="36" t="s">
         <v>846</v>
       </c>
       <c r="R44" s="26"/>
@@ -9379,7 +9379,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="60.75" thickBot="1">
+    <row r="52" spans="1:20" ht="90.75" thickBot="1">
       <c r="A52" s="20">
         <v>45</v>
       </c>
@@ -9399,7 +9399,7 @@
         <v>45194</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="H52" s="24"/>
       <c r="I52" s="24"/>
@@ -9407,22 +9407,22 @@
         <v>139</v>
       </c>
       <c r="K52" s="25"/>
-      <c r="L52" s="48" t="s">
+      <c r="L52" s="36" t="s">
         <v>848</v>
       </c>
-      <c r="M52" s="48" t="s">
+      <c r="M52" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="N52" s="48" t="s">
-        <v>888</v>
-      </c>
-      <c r="O52" s="48" t="s">
+      <c r="N52" s="36" t="s">
+        <v>882</v>
+      </c>
+      <c r="O52" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="P52" s="49" t="s">
-        <v>891</v>
-      </c>
-      <c r="Q52" s="48" t="s">
+      <c r="P52" s="37" t="s">
+        <v>885</v>
+      </c>
+      <c r="Q52" s="36" t="s">
         <v>846</v>
       </c>
       <c r="R52" s="26" t="s">
@@ -10047,9 +10047,9 @@
         <v>848</v>
       </c>
       <c r="K70" s="25" t="s">
-        <v>865</v>
-      </c>
-      <c r="L70" s="48"/>
+        <v>859</v>
+      </c>
+      <c r="L70" s="36"/>
       <c r="M70" s="25"/>
       <c r="N70" s="25"/>
       <c r="O70" s="25"/>
@@ -10085,9 +10085,9 @@
         <v>848</v>
       </c>
       <c r="K71" s="25" t="s">
-        <v>866</v>
-      </c>
-      <c r="L71" s="48"/>
+        <v>860</v>
+      </c>
+      <c r="L71" s="36"/>
       <c r="M71" s="25"/>
       <c r="N71" s="25"/>
       <c r="O71" s="25"/>
@@ -10119,34 +10119,34 @@
         <v>45194</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="J72" s="25" t="s">
         <v>139</v>
       </c>
       <c r="K72" s="25"/>
-      <c r="L72" s="48" t="s">
+      <c r="L72" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="M72" s="48" t="s">
+      <c r="M72" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="N72" s="48" t="s">
-        <v>889</v>
-      </c>
-      <c r="O72" s="48" t="s">
+      <c r="N72" s="36" t="s">
+        <v>883</v>
+      </c>
+      <c r="O72" s="36" t="s">
         <v>848</v>
       </c>
-      <c r="P72" s="49" t="s">
-        <v>892</v>
-      </c>
-      <c r="Q72" s="48" t="s">
+      <c r="P72" s="37" t="s">
+        <v>886</v>
+      </c>
+      <c r="Q72" s="36" t="s">
         <v>846</v>
       </c>
       <c r="R72" s="26"/>
@@ -10179,9 +10179,9 @@
         <v>848</v>
       </c>
       <c r="K73" s="25" t="s">
-        <v>870</v>
-      </c>
-      <c r="L73" s="48"/>
+        <v>864</v>
+      </c>
+      <c r="L73" s="36"/>
       <c r="M73" s="25"/>
       <c r="N73" s="25"/>
       <c r="O73" s="25"/>
@@ -10213,34 +10213,34 @@
         <v>45194</v>
       </c>
       <c r="G74" s="24" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="H74" s="24" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="I74" s="24" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
       <c r="J74" s="25" t="s">
         <v>139</v>
       </c>
       <c r="K74" s="25"/>
-      <c r="L74" s="48" t="s">
+      <c r="L74" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="M74" s="48" t="s">
+      <c r="M74" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="N74" s="48" t="s">
-        <v>889</v>
-      </c>
-      <c r="O74" s="48" t="s">
+      <c r="N74" s="36" t="s">
+        <v>883</v>
+      </c>
+      <c r="O74" s="36" t="s">
         <v>848</v>
       </c>
-      <c r="P74" s="49" t="s">
-        <v>892</v>
-      </c>
-      <c r="Q74" s="48" t="s">
+      <c r="P74" s="37" t="s">
+        <v>886</v>
+      </c>
+      <c r="Q74" s="36" t="s">
         <v>846</v>
       </c>
       <c r="R74" s="26"/>
@@ -10269,34 +10269,34 @@
         <v>45194</v>
       </c>
       <c r="G75" s="24" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
       <c r="H75" s="24" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="I75" s="24" t="s">
-        <v>876</v>
+        <v>870</v>
       </c>
       <c r="J75" s="25" t="s">
         <v>139</v>
       </c>
       <c r="K75" s="25"/>
-      <c r="L75" s="48" t="s">
+      <c r="L75" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="M75" s="48" t="s">
+      <c r="M75" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="N75" s="48" t="s">
-        <v>889</v>
-      </c>
-      <c r="O75" s="48" t="s">
+      <c r="N75" s="36" t="s">
+        <v>883</v>
+      </c>
+      <c r="O75" s="36" t="s">
         <v>848</v>
       </c>
-      <c r="P75" s="49" t="s">
-        <v>892</v>
-      </c>
-      <c r="Q75" s="48" t="s">
+      <c r="P75" s="37" t="s">
+        <v>886</v>
+      </c>
+      <c r="Q75" s="36" t="s">
         <v>846</v>
       </c>
       <c r="R75" s="26"/>
@@ -10325,34 +10325,34 @@
         <v>45194</v>
       </c>
       <c r="G76" s="24" t="s">
-        <v>878</v>
+        <v>872</v>
       </c>
       <c r="H76" s="24" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
       <c r="I76" s="24" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="J76" s="25" t="s">
         <v>139</v>
       </c>
       <c r="K76" s="25"/>
-      <c r="L76" s="48" t="s">
+      <c r="L76" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="M76" s="48" t="s">
+      <c r="M76" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="N76" s="48" t="s">
-        <v>889</v>
-      </c>
-      <c r="O76" s="48" t="s">
+      <c r="N76" s="36" t="s">
+        <v>883</v>
+      </c>
+      <c r="O76" s="36" t="s">
         <v>848</v>
       </c>
-      <c r="P76" s="49" t="s">
-        <v>892</v>
-      </c>
-      <c r="Q76" s="48" t="s">
+      <c r="P76" s="37" t="s">
+        <v>886</v>
+      </c>
+      <c r="Q76" s="36" t="s">
         <v>846</v>
       </c>
       <c r="R76" s="26"/>
@@ -10381,34 +10381,34 @@
         <v>45194</v>
       </c>
       <c r="G77" s="24" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="H77" s="24" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="I77" s="24" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="J77" s="25" t="s">
         <v>139</v>
       </c>
       <c r="K77" s="25"/>
-      <c r="L77" s="48" t="s">
+      <c r="L77" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="M77" s="48" t="s">
+      <c r="M77" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="N77" s="48" t="s">
-        <v>889</v>
-      </c>
-      <c r="O77" s="48" t="s">
+      <c r="N77" s="36" t="s">
+        <v>883</v>
+      </c>
+      <c r="O77" s="36" t="s">
         <v>848</v>
       </c>
-      <c r="P77" s="49" t="s">
-        <v>892</v>
-      </c>
-      <c r="Q77" s="48" t="s">
+      <c r="P77" s="37" t="s">
+        <v>886</v>
+      </c>
+      <c r="Q77" s="36" t="s">
         <v>846</v>
       </c>
       <c r="R77" s="26"/>
@@ -10441,9 +10441,9 @@
         <v>848</v>
       </c>
       <c r="K78" s="25" t="s">
-        <v>877</v>
-      </c>
-      <c r="L78" s="48"/>
+        <v>871</v>
+      </c>
+      <c r="L78" s="36"/>
       <c r="M78" s="25"/>
       <c r="N78" s="25"/>
       <c r="O78" s="25"/>
@@ -10479,9 +10479,9 @@
         <v>848</v>
       </c>
       <c r="K79" s="25" t="s">
-        <v>877</v>
-      </c>
-      <c r="L79" s="48"/>
+        <v>871</v>
+      </c>
+      <c r="L79" s="36"/>
       <c r="M79" s="25"/>
       <c r="N79" s="25"/>
       <c r="O79" s="25"/>
@@ -10513,34 +10513,34 @@
         <v>45194</v>
       </c>
       <c r="G80" s="24" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="H80" s="24" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="I80" s="24" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="J80" s="25" t="s">
         <v>139</v>
       </c>
       <c r="K80" s="25"/>
-      <c r="L80" s="48" t="s">
+      <c r="L80" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="M80" s="48" t="s">
+      <c r="M80" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="N80" s="48" t="s">
-        <v>890</v>
-      </c>
-      <c r="O80" s="48" t="s">
+      <c r="N80" s="36" t="s">
+        <v>884</v>
+      </c>
+      <c r="O80" s="36" t="s">
         <v>848</v>
       </c>
-      <c r="P80" s="49" t="s">
-        <v>892</v>
-      </c>
-      <c r="Q80" s="48" t="s">
+      <c r="P80" s="37" t="s">
+        <v>886</v>
+      </c>
+      <c r="Q80" s="36" t="s">
         <v>846</v>
       </c>
       <c r="R80" s="26"/>
@@ -10573,9 +10573,9 @@
         <v>848</v>
       </c>
       <c r="K81" s="25" t="s">
-        <v>877</v>
-      </c>
-      <c r="L81" s="48"/>
+        <v>871</v>
+      </c>
+      <c r="L81" s="36"/>
       <c r="M81" s="25"/>
       <c r="N81" s="25"/>
       <c r="O81" s="25"/>
@@ -20600,16 +20600,16 @@
         <v>780</v>
       </c>
       <c r="F376" s="23">
-        <v>45194</v>
+        <v>45208</v>
       </c>
       <c r="G376" s="24" t="s">
-        <v>861</v>
+        <v>890</v>
       </c>
       <c r="H376" s="24" t="s">
-        <v>862</v>
+        <v>891</v>
       </c>
       <c r="I376" s="24" t="s">
-        <v>863</v>
+        <v>892</v>
       </c>
       <c r="J376" s="25" t="s">
         <v>139</v>
@@ -20620,7 +20620,7 @@
       <c r="N376" s="25"/>
       <c r="O376" s="25"/>
       <c r="P376" s="25"/>
-      <c r="Q376" s="48" t="s">
+      <c r="Q376" s="36" t="s">
         <v>846</v>
       </c>
       <c r="R376" s="26"/>

</xml_diff>